<commit_message>
Add solar_cost in route
</commit_message>
<xml_diff>
--- a/storage/app/report-template/route.xlsx
+++ b/storage/app/report-template/route.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Master Data Rute</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">Komisi Kenek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tambahan Solar</t>
   </si>
   <si>
     <t xml:space="preserve">Aktif</t>
@@ -251,25 +254,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.1943319838057"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="17.9676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="2" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
@@ -289,6 +307,9 @@
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +318,8 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Adjust route export to include price
</commit_message>
<xml_diff>
--- a/storage/app/report-template/route.xlsx
+++ b/storage/app/report-template/route.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farizhermawan/other/jmp-tracking-ho-be/storage/app/report-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD20B0D-E5A7-A14F-A9F2-16E0080A7919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9760D32-2C54-BE45-ACD5-394449D4B4CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Master Data Rute</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Aktif</t>
+  </si>
+  <si>
+    <t>Harga Jual</t>
   </si>
 </sst>
 </file>
@@ -521,22 +524,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.33203125" style="1"/>
     <col min="2" max="2" width="32.5" style="1"/>
-    <col min="3" max="6" width="18.1640625" style="2"/>
-    <col min="7" max="7" width="9.1640625" style="3"/>
-    <col min="8" max="1025" width="9.1640625"/>
+    <col min="3" max="3" width="21.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" style="2" customWidth="1"/>
+    <col min="5" max="7" width="18.1640625" style="2"/>
+    <col min="8" max="8" width="9.1640625" style="3"/>
+    <col min="9" max="1026" width="9.1640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -546,8 +551,9 @@
       <c r="E1"/>
       <c r="F1"/>
       <c r="G1"/>
+      <c r="H1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
@@ -555,8 +561,9 @@
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
+      <c r="H2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -564,29 +571,33 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>